<commit_message>
added data labels to word count viz
</commit_message>
<xml_diff>
--- a/emily data.xlsx
+++ b/emily data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jenwh\Documents\nss\projects\sql-assessment-jenwhitson\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53A69E20-F5CD-4812-8369-F27A4C676A42}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09AEB711-01BC-429C-AC00-6624EBDF9FED}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="viz" sheetId="3" r:id="rId1"/>
@@ -1544,6 +1544,60 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent1">
+                          <a:lumMod val="60000"/>
+                          <a:lumOff val="40000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>'emily data'!$A$2:$A$6</c:f>
@@ -4450,8 +4504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:O23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N31" sqref="N31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4599,7 +4653,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>

</xml_diff>